<commit_message>
2020_12_12 merge mobile qpyton project directory
</commit_message>
<xml_diff>
--- a/github_cmds.xlsx
+++ b/github_cmds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C090277-F475-FC4F-9008-81B67CA3E6DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86A58E67-BA89-9E41-AE16-AD662F71117F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="2295" windowWidth="16245" windowHeight="12705" xr2:uid="{8F2625FD-89A9-4B3D-8A00-8DF7F9DA0750}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>SSH</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>If you want to clone the repository into a directory named something other than libgit2, you can specify the new directory name as an additional argument:</t>
+  </si>
+  <si>
+    <t>Unmodifying a Modified File</t>
+  </si>
+  <si>
+    <t>$ git checkout -- CONTRIBUTING.md</t>
+  </si>
+  <si>
+    <t>Unmodifying a Modified File with git restore</t>
+  </si>
+  <si>
+    <t>$ git restore CONTRIBUTING.md</t>
   </si>
 </sst>
 </file>
@@ -607,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDC9B31-712E-4E5B-94AD-D272F284797C}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -731,119 +743,135 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" xr:uid="{C7519BB9-4990-4441-85D8-3F8D734486E5}"/>
-    <hyperlink ref="C21" r:id="rId2" xr:uid="{F79C6C8A-CBC0-431B-9513-8B085982791B}"/>
-    <hyperlink ref="C23" r:id="rId3" xr:uid="{DE5C9EB2-D030-4578-8F80-4966C6FB18CC}"/>
-    <hyperlink ref="C29" r:id="rId4" xr:uid="{1215AFF7-7BD6-48B5-8901-225043A459B0}"/>
+    <hyperlink ref="C29" r:id="rId1" xr:uid="{C7519BB9-4990-4441-85D8-3F8D734486E5}"/>
+    <hyperlink ref="C23" r:id="rId2" xr:uid="{F79C6C8A-CBC0-431B-9513-8B085982791B}"/>
+    <hyperlink ref="C25" r:id="rId3" xr:uid="{DE5C9EB2-D030-4578-8F80-4966C6FB18CC}"/>
+    <hyperlink ref="C31" r:id="rId4" xr:uid="{1215AFF7-7BD6-48B5-8901-225043A459B0}"/>
     <hyperlink ref="C3" r:id="rId5" xr:uid="{5C62FD82-4872-4EC9-A92A-846A76165160}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{FC56FECA-2CD4-4887-9580-C401BD487AA1}"/>
     <hyperlink ref="C17" r:id="rId7" xr:uid="{E597F76D-D8BF-43D2-9023-C2BC6BEEF4BD}"/>
-    <hyperlink ref="C18" r:id="rId8" xr:uid="{BD695441-FA05-4A8D-97D7-1774ABEAEF28}"/>
+    <hyperlink ref="C20" r:id="rId8" xr:uid="{BD695441-FA05-4A8D-97D7-1774ABEAEF28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>